<commit_message>
Adicionando alterações na página sobre, na biblioteca e no login e cadastro.
</commit_message>
<xml_diff>
--- a/Documentação/Backlogs e Burndown/Backlog - Jurubeba Blues.xlsx
+++ b/Documentação/Backlogs e Burndown/Backlog - Jurubeba Blues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fc61e1cbd89c56e/Área de Trabalho/Projeto Individual/Documentação/Backlogs e Burndown/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fc61e1cbd89c56e/Área de Trabalho/Projeto-Individual/Documentação/Backlogs e Burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{5BB3E342-6D0F-4D25-AF04-2A00E99CD59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9049714E-4B3D-46A5-ABEC-A4E29C91CC5C}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{5BB3E342-6D0F-4D25-AF04-2A00E99CD59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F75DB72-66BB-4438-B7B6-F0C9918E9F39}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FBC5F0C2-FC0E-44A3-835F-69213FEE4454}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FBC5F0C2-FC0E-44A3-835F-69213FEE4454}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>SPRINT</t>
   </si>
@@ -103,15 +103,6 @@
     <t>Armazenamento no banco de dados</t>
   </si>
   <si>
-    <t>Diagrama de solução</t>
-  </si>
-  <si>
-    <t>Diagrama de negócios</t>
-  </si>
-  <si>
-    <t>Planilha de Riscos</t>
-  </si>
-  <si>
     <t>Site institucional funcional</t>
   </si>
   <si>
@@ -155,15 +146,6 @@
   </si>
   <si>
     <t>Processo de salvar, recuperar e gerenciar dados no banco (como MySQL, PostgreSQL, MongoDB etc.), garantindo persistência das informações.</t>
-  </si>
-  <si>
-    <t>Representação gráfica da arquitetura técnica da aplicação, incluindo fluxos de dados, componentes do sistema e interações entre eles</t>
-  </si>
-  <si>
-    <t>Mapeamento visual dos processos de negócio envolvidos no projeto, evidenciando como as funções do sistema se alinham aos objetivos do usuário.</t>
-  </si>
-  <si>
-    <t>Documento que identifica possíveis riscos no projeto, sua gravidade, probabilidade e planos de mitigação.</t>
   </si>
   <si>
     <t>Versão em funcionamento do site institucional com conteúdo, navegação e funcionalidades básicas acessíveis ao público.</t>
@@ -273,20 +255,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,14 +611,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C78C8B2-FB08-48E1-9688-9446C15C8180}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" customWidth="1"/>
@@ -644,433 +626,391 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="E10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>21</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="D12" s="5">
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5">
+        <v>21</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="F13" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="G13" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="F14" s="5">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6">
-        <v>21</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="F15" s="5">
         <v>2</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6">
-        <v>21</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="G15" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5">
+        <v>13</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="5">
         <v>2</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6">
-        <v>5</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="6">
-        <v>3</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="6">
-        <v>3</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6">
-        <v>5</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="6">
-        <v>3</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6">
-        <v>21</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>13</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6">
-        <v>21</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="6">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="6">
-        <v>13</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="6">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="G16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="6">
-        <v>21</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="6">
-        <v>3</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="17" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="6">
-        <v>13</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="6">
-        <v>3</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="6">
-        <v>5</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="6">
-        <v>2</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="6">
-        <v>13</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="6">
-        <v>2</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="4"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1079,7 +1019,7 @@
     </row>
     <row r="21" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1088,7 +1028,7 @@
     </row>
     <row r="22" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="4"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1097,7 +1037,7 @@
     </row>
     <row r="23" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="4"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1106,7 +1046,7 @@
     </row>
     <row r="24" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1115,40 +1055,16 @@
     </row>
     <row r="25" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
+    <row r="26" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
@@ -1168,7 +1084,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1188,7 +1104,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>